<commit_message>
Removed Base64 coded files.
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/ChangeConclusions.xlsx
+++ b/BloodstreamAPI/testData/ChangeConclusions.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC48E60-DB43-4771-8184-4625606876EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8120BDBD-7AB3-451C-9079-F2BB66393611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChangetoUntested" sheetId="7" r:id="rId1"/>
+    <sheet name="ChangeAnyConclusions" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>EndPoint</t>
   </si>
@@ -35,6 +36,9 @@
   </si>
   <si>
     <t>/conclusions/invalidateAndApprove</t>
+  </si>
+  <si>
+    <t>/conclusions/changeAndApprove</t>
   </si>
 </sst>
 </file>
@@ -396,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FC9B42-5356-4D66-ABF8-4EF2DFAF1ABA}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,4 +535,155 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB86F7E-1E62-4CB0-99B3-BFFF33B060A2}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A14:E14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>